<commit_message>
change the excel file
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -79,12 +79,6 @@
     <t>kennethedwardsee@gmail.com</t>
   </si>
   <si>
-    <t>pastorheidi@wfcrc.ca</t>
-  </si>
-  <si>
-    <t>Pastor Rev Heidi</t>
-  </si>
-  <si>
     <t>Jeff_Shrum@sil.org</t>
   </si>
   <si>
@@ -146,13 +140,19 @@
   </si>
   <si>
     <t>495-9548</t>
+  </si>
+  <si>
+    <t>Ken M</t>
+  </si>
+  <si>
+    <t>Ken_Mullins@sil.org</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +284,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -586,7 +594,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -629,11 +637,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -667,6 +677,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -977,7 +988,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,13 +1000,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1006,7 +1017,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,7 +1028,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1028,7 +1039,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1039,7 +1050,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1050,7 +1061,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1061,7 +1072,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1072,7 +1083,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1083,7 +1094,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1094,18 +1105,18 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1116,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1124,46 +1135,49 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>